<commit_message>
switched to Geneva investment positions report, tested OK
</commit_message>
<xml_diff>
--- a/samples/DIF_20200429_investment_position.xlsx
+++ b/samples/DIF_20200429_investment_position.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\git\risk_report\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CB1F9B-73E6-4D7D-BC2F-9CA649A5F832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4DBBDE-AB90-4427-9EC4-9463B042F977}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31710" yWindow="375" windowWidth="21960" windowHeight="14850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report Investment Position Appr" sheetId="1" r:id="rId1"/>
@@ -2453,27 +2453,27 @@
   <dimension ref="A1:O311"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C258" sqref="C258"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.5546875" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>2.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>1.3899999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>5.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>2.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>1.72E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>4.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>5.3E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>3.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>1.38E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -3708,7 +3708,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>5.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>2.12E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>1.6899999999999998E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>9.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>1.72E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>1.04E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>3.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>1.83E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -4324,7 +4324,7 @@
         <v>5.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>1.03E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>15</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -4544,7 +4544,7 @@
         <v>9.4000000000000004E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>15</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>5.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>8.6E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>1.12E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -4940,7 +4940,7 @@
         <v>1.9300000000000001E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -4984,7 +4984,7 @@
         <v>5.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -5028,7 +5028,7 @@
         <v>2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>15</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>15</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>15</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>1.1900000000000001E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>2.5399999999999999E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>15</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>15</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>15</v>
       </c>
@@ -5468,7 +5468,7 @@
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -5512,7 +5512,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>15</v>
       </c>
@@ -5556,7 +5556,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>15</v>
       </c>
@@ -5600,7 +5600,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>15</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>15</v>
       </c>
@@ -5732,7 +5732,7 @@
         <v>1.61E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>15</v>
       </c>
@@ -5776,7 +5776,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>15</v>
       </c>
@@ -5820,7 +5820,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>1.0800000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>15</v>
       </c>
@@ -5996,7 +5996,7 @@
         <v>4.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>15</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>8.3999999999999995E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>15</v>
       </c>
@@ -6084,7 +6084,7 @@
         <v>4.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>15</v>
       </c>
@@ -6128,7 +6128,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>15</v>
       </c>
@@ -6172,7 +6172,7 @@
         <v>2.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>15</v>
       </c>
@@ -6216,7 +6216,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>15</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>15</v>
       </c>
@@ -6304,7 +6304,7 @@
         <v>2.1299999999999999E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>15</v>
       </c>
@@ -6348,7 +6348,7 @@
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>15</v>
       </c>
@@ -6392,7 +6392,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>15</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>15</v>
       </c>
@@ -6480,7 +6480,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>15</v>
       </c>
@@ -6524,7 +6524,7 @@
         <v>5.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>15</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>15</v>
       </c>
@@ -6612,7 +6612,7 @@
         <v>3.3E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>15</v>
       </c>
@@ -6656,7 +6656,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>15</v>
       </c>
@@ -6700,7 +6700,7 @@
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>15</v>
       </c>
@@ -6744,7 +6744,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>15</v>
       </c>
@@ -6788,7 +6788,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>15</v>
       </c>
@@ -6832,7 +6832,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>15</v>
       </c>
@@ -6876,7 +6876,7 @@
         <v>2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>15</v>
       </c>
@@ -6920,7 +6920,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>15</v>
       </c>
@@ -6964,7 +6964,7 @@
         <v>2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>15</v>
       </c>
@@ -7008,7 +7008,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>15</v>
       </c>
@@ -7052,7 +7052,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>15</v>
       </c>
@@ -7096,7 +7096,7 @@
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>15</v>
       </c>
@@ -7140,7 +7140,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>15</v>
       </c>
@@ -7184,7 +7184,7 @@
         <v>8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>15</v>
       </c>
@@ -7228,7 +7228,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>15</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>1.43E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>15</v>
       </c>
@@ -7316,7 +7316,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>15</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>15</v>
       </c>
@@ -7404,7 +7404,7 @@
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>15</v>
       </c>
@@ -7448,7 +7448,7 @@
         <v>2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>15</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>15</v>
       </c>
@@ -7536,7 +7536,7 @@
         <v>7.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>15</v>
       </c>
@@ -7580,7 +7580,7 @@
         <v>5.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>15</v>
       </c>
@@ -7624,7 +7624,7 @@
         <v>2.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>15</v>
       </c>
@@ -7668,7 +7668,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>15</v>
       </c>
@@ -7712,7 +7712,7 @@
         <v>3.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>15</v>
       </c>
@@ -7756,7 +7756,7 @@
         <v>3.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>15</v>
       </c>
@@ -7800,7 +7800,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>15</v>
       </c>
@@ -7844,7 +7844,7 @@
         <v>1.4200000000000001E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>15</v>
       </c>
@@ -7888,7 +7888,7 @@
         <v>3.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>15</v>
       </c>
@@ -7932,7 +7932,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>15</v>
       </c>
@@ -7976,7 +7976,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>15</v>
       </c>
@@ -8020,7 +8020,7 @@
         <v>9.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>15</v>
       </c>
@@ -8064,7 +8064,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>15</v>
       </c>
@@ -8108,7 +8108,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>15</v>
       </c>
@@ -8152,7 +8152,7 @@
         <v>6.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>15</v>
       </c>
@@ -8196,7 +8196,7 @@
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>15</v>
       </c>
@@ -8240,7 +8240,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>15</v>
       </c>
@@ -8284,7 +8284,7 @@
         <v>8.2000000000000007E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>15</v>
       </c>
@@ -8328,7 +8328,7 @@
         <v>2.3E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>15</v>
       </c>
@@ -8372,7 +8372,7 @@
         <v>1.06E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>15</v>
       </c>
@@ -8416,7 +8416,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>15</v>
       </c>
@@ -8460,7 +8460,7 @@
         <v>5.3E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>15</v>
       </c>
@@ -8504,7 +8504,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>15</v>
       </c>
@@ -8548,7 +8548,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>15</v>
       </c>
@@ -8592,7 +8592,7 @@
         <v>8.8000000000000005E-3</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>15</v>
       </c>
@@ -8636,7 +8636,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>15</v>
       </c>
@@ -8680,7 +8680,7 @@
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>15</v>
       </c>
@@ -8724,7 +8724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>15</v>
       </c>
@@ -8768,7 +8768,7 @@
         <v>5.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>15</v>
       </c>
@@ -8812,7 +8812,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>15</v>
       </c>
@@ -8856,7 +8856,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>15</v>
       </c>
@@ -8900,7 +8900,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>15</v>
       </c>
@@ -8944,7 +8944,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>15</v>
       </c>
@@ -8988,7 +8988,7 @@
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>15</v>
       </c>
@@ -9032,7 +9032,7 @@
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>15</v>
       </c>
@@ -9076,7 +9076,7 @@
         <v>6.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>15</v>
       </c>
@@ -9120,7 +9120,7 @@
         <v>4.1999999999999997E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>15</v>
       </c>
@@ -9164,7 +9164,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>15</v>
       </c>
@@ -9208,7 +9208,7 @@
         <v>2.3599999999999999E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>15</v>
       </c>
@@ -9252,7 +9252,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>15</v>
       </c>
@@ -9296,7 +9296,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>15</v>
       </c>
@@ -9340,7 +9340,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>15</v>
       </c>
@@ -9384,7 +9384,7 @@
         <v>8.6E-3</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>15</v>
       </c>
@@ -9428,7 +9428,7 @@
         <v>3.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>15</v>
       </c>
@@ -9472,7 +9472,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>15</v>
       </c>
@@ -9516,7 +9516,7 @@
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>15</v>
       </c>
@@ -9560,7 +9560,7 @@
         <v>3.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>15</v>
       </c>
@@ -9604,7 +9604,7 @@
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>15</v>
       </c>
@@ -9648,7 +9648,7 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>15</v>
       </c>
@@ -9692,7 +9692,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>15</v>
       </c>
@@ -9736,7 +9736,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>15</v>
       </c>
@@ -9780,7 +9780,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>15</v>
       </c>
@@ -9824,7 +9824,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>15</v>
       </c>
@@ -9868,7 +9868,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>15</v>
       </c>
@@ -9912,7 +9912,7 @@
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>15</v>
       </c>
@@ -9956,7 +9956,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>15</v>
       </c>
@@ -10000,7 +10000,7 @@
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>15</v>
       </c>
@@ -10044,7 +10044,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>15</v>
       </c>
@@ -10088,7 +10088,7 @@
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>15</v>
       </c>
@@ -10132,7 +10132,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>15</v>
       </c>
@@ -10176,7 +10176,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>15</v>
       </c>
@@ -10220,7 +10220,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>15</v>
       </c>
@@ -10264,7 +10264,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>15</v>
       </c>
@@ -10308,7 +10308,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>15</v>
       </c>
@@ -10352,7 +10352,7 @@
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>15</v>
       </c>
@@ -10396,7 +10396,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>383</v>
       </c>
@@ -10440,7 +10440,7 @@
         <v>-5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>383</v>
       </c>
@@ -10484,7 +10484,7 @@
         <v>-1E-4</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>383</v>
       </c>
@@ -10528,7 +10528,7 @@
         <v>1.0005999999999999</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>387</v>
       </c>
@@ -10572,7 +10572,7 @@
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>387</v>
       </c>
@@ -10616,7 +10616,7 @@
         <v>8.9399999999999993E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>387</v>
       </c>
@@ -10660,7 +10660,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>387</v>
       </c>
@@ -10704,7 +10704,7 @@
         <v>3.7900000000000003E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>387</v>
       </c>
@@ -10748,7 +10748,7 @@
         <v>0.85150000000000003</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>387</v>
       </c>
@@ -10792,7 +10792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>387</v>
       </c>
@@ -10836,7 +10836,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>387</v>
       </c>
@@ -10880,7 +10880,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>387</v>
       </c>
@@ -10924,7 +10924,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>387</v>
       </c>
@@ -10968,7 +10968,7 @@
         <v>1.5800000000000002E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>398</v>
       </c>
@@ -10976,7 +10976,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>400</v>
       </c>
@@ -10984,12 +10984,12 @@
         <v>19437</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>402</v>
       </c>
@@ -10997,17 +10997,17 @@
         <v>403</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>406</v>
       </c>
@@ -11015,12 +11015,12 @@
         <v>407</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>409</v>
       </c>
@@ -11028,7 +11028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>410</v>
       </c>
@@ -11036,7 +11036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>411</v>
       </c>
@@ -11044,7 +11044,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>413</v>
       </c>
@@ -11052,7 +11052,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>415</v>
       </c>
@@ -11060,7 +11060,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>417</v>
       </c>
@@ -11068,67 +11068,67 @@
         <v>18264</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>430</v>
       </c>
@@ -11136,7 +11136,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>432</v>
       </c>
@@ -11144,7 +11144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>433</v>
       </c>
@@ -11152,7 +11152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>434</v>
       </c>
@@ -11160,7 +11160,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>436</v>
       </c>
@@ -11168,7 +11168,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>437</v>
       </c>
@@ -11176,7 +11176,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>439</v>
       </c>
@@ -11184,7 +11184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>440</v>
       </c>
@@ -11192,7 +11192,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>442</v>
       </c>
@@ -11200,12 +11200,12 @@
         <v>443</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>445</v>
       </c>
@@ -11213,7 +11213,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>446</v>
       </c>
@@ -11221,7 +11221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>447</v>
       </c>
@@ -11229,7 +11229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>448</v>
       </c>
@@ -11237,7 +11237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>449</v>
       </c>
@@ -11245,7 +11245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>450</v>
       </c>
@@ -11253,7 +11253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>451</v>
       </c>
@@ -11261,7 +11261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>452</v>
       </c>
@@ -11269,7 +11269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>453</v>
       </c>
@@ -11277,7 +11277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>454</v>
       </c>
@@ -11285,7 +11285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>455</v>
       </c>
@@ -11293,7 +11293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>456</v>
       </c>
@@ -11301,7 +11301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>457</v>
       </c>
@@ -11309,7 +11309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>458</v>
       </c>
@@ -11317,7 +11317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>459</v>
       </c>
@@ -11325,7 +11325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>460</v>
       </c>
@@ -11333,7 +11333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>461</v>
       </c>
@@ -11341,7 +11341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>462</v>
       </c>
@@ -11349,7 +11349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>463</v>
       </c>
@@ -11357,17 +11357,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>466</v>
       </c>
@@ -11375,7 +11375,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>467</v>
       </c>
@@ -11383,7 +11383,7 @@
         <v>19437</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>468</v>
       </c>
@@ -11391,12 +11391,12 @@
         <v>469</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>471</v>
       </c>
@@ -11404,7 +11404,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>473</v>
       </c>
@@ -11412,12 +11412,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>475</v>
       </c>
@@ -11425,7 +11425,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>477</v>
       </c>
@@ -11433,7 +11433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>478</v>
       </c>
@@ -11441,7 +11441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>479</v>
       </c>
@@ -11449,7 +11449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>480</v>
       </c>
@@ -11457,7 +11457,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>482</v>
       </c>
@@ -11465,12 +11465,12 @@
         <v>483</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>485</v>
       </c>
@@ -11478,12 +11478,12 @@
         <v>43976.465219907404</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>487</v>
       </c>
@@ -11491,7 +11491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>488</v>
       </c>
@@ -11499,7 +11499,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>490</v>
       </c>
@@ -11507,7 +11507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>491</v>
       </c>
@@ -11515,12 +11515,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>493</v>
       </c>
@@ -11528,12 +11528,12 @@
         <v>494</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>496</v>
       </c>
@@ -11541,12 +11541,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>498</v>
       </c>
@@ -11554,7 +11554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>499</v>
       </c>
@@ -11562,7 +11562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>500</v>
       </c>
@@ -11570,7 +11570,7 @@
         <v>43950.999988425923</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>501</v>
       </c>
@@ -11578,7 +11578,7 @@
         <v>18264</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>502</v>
       </c>
@@ -11586,7 +11586,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>504</v>
       </c>
@@ -11594,7 +11594,7 @@
         <v>19437</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>505</v>
       </c>
@@ -11602,7 +11602,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>506</v>
       </c>
@@ -11610,7 +11610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>507</v>
       </c>
@@ -11618,7 +11618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>508</v>
       </c>
@@ -11626,7 +11626,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>510</v>
       </c>
@@ -11634,7 +11634,7 @@
         <v>43976</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>511</v>
       </c>
@@ -11642,12 +11642,12 @@
         <v>512</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>514</v>
       </c>
@@ -11655,7 +11655,7 @@
         <v>50041</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>515</v>
       </c>
@@ -11663,27 +11663,27 @@
         <v>516</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>521</v>
       </c>
@@ -11691,7 +11691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>443</v>
       </c>
@@ -11699,7 +11699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>522</v>
       </c>
@@ -11707,7 +11707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>523</v>
       </c>
@@ -11715,22 +11715,22 @@
         <v>524</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>528</v>
       </c>
@@ -11738,12 +11738,12 @@
         <v>529</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>531</v>
       </c>
@@ -11751,7 +11751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>398</v>
       </c>
@@ -11759,7 +11759,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>532</v>
       </c>
@@ -11767,7 +11767,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>534</v>
       </c>
@@ -11775,7 +11775,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>19044</v>
       </c>

</xml_diff>